<commit_message>
corrected links on strike table. found small mistake. now I do weekend and go play football with my son
</commit_message>
<xml_diff>
--- a/utils/germany_strikedata.xlsx
+++ b/utils/germany_strikedata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f6d213be512b1d25/DS FHNW/FS25/wer/OMC/simulation_of_the_delivery_time/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexi\OneDrive\DS FHNW\2_FS_25\wer\OMC\simulation_of_the_delivery_time\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="243" documentId="13_ncr:1_{3E920921-FE47-4E07-A11E-8BD7E105E9BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CF07CD3-8A8B-4E3C-8641-5981F9AABEB0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10008F9D-6F26-4234-82F3-27FDACEBFFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{D19E7103-73BE-4B4C-956A-9FE499A31348}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="80">
   <si>
     <t xml:space="preserve">logistik strikes in germany 2014 -2024 </t>
   </si>
@@ -119,9 +119,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>https://www.reuters.com/</t>
-  </si>
-  <si>
     <t>Phased Lufthansa pilot strike. Some cargo flights cancelled</t>
   </si>
   <si>
@@ -131,15 +128,9 @@
     <t>Nationwide Deutsche Post strike. 15% of letters and 25% of parcels delayed. Took 2–3 weeks to recover.</t>
   </si>
   <si>
-    <t>https://www.sueddeutsche.de/</t>
-  </si>
-  <si>
     <t>Three waves of GDL strikes; 265 hours total. Delays for industrial cargo, recovery over several days.</t>
   </si>
   <si>
-    <t>https://www.dbcargo.com/</t>
-  </si>
-  <si>
     <t>factored</t>
   </si>
   <si>
@@ -161,18 +152,12 @@
     <t>Short warning strike. Port operations paused for one shift.</t>
   </si>
   <si>
-    <t>https://www.trans.info/</t>
-  </si>
-  <si>
     <t>2022 14–16 Jul</t>
   </si>
   <si>
     <t>48h North Sea port strike. 20+ ships delayed. Backlog took up to 2 weeks to clear.</t>
   </si>
   <si>
-    <t>https://www.abendblatt.de/</t>
-  </si>
-  <si>
     <t xml:space="preserve">2022 2 Sep </t>
   </si>
   <si>
@@ -185,9 +170,6 @@
     <t>Series of short warning strikes. Local delays, recovered in 1–2 days each.</t>
   </si>
   <si>
-    <t>https://www.mdr.de/</t>
-  </si>
-  <si>
     <t>sources</t>
   </si>
   <si>
@@ -197,9 +179,6 @@
     <t>24h EVG warning strike. All DB freight halted. 1–2 day delays for shipments.</t>
   </si>
   <si>
-    <t>https://www.tagesschau.de/</t>
-  </si>
-  <si>
     <t>2023 27 Mar</t>
   </si>
   <si>
@@ -216,9 +195,6 @@
   </si>
   <si>
     <t>Lufthansa Cargo ground staff strike. Five freighter flights cancelled, 1–3 day backlog.</t>
-  </si>
-  <si>
-    <t>https://www.hessenschau.de/</t>
   </si>
   <si>
     <t>Sum</t>
@@ -261,9 +237,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Gestutzes Mittel oder Werte von 0.5 bis 3 verwenden?</t>
-  </si>
-  <si>
     <t>Gestutzes Mittel</t>
   </si>
   <si>
@@ -325,9 +298,6 @@
     </r>
   </si>
   <si>
-    <t>Artihemtisches Mittel oder Modalwert hier besser geeignet?</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -418,9 +388,6 @@
     </r>
   </si>
   <si>
-    <t>Wieviele Kommastellen?</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">43 / 5 = </t>
     </r>
@@ -454,6 +421,39 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>https://www.sueddeutsche.de/wirtschaft/streik-bei-der-post-sag-mir-wo-die-briefe-sind-1.2512685</t>
+  </si>
+  <si>
+    <t>https://www.reuters.com/article/2015/03/21/us-lufthansa-strikes-idUSKBN0MH09820150321/</t>
+  </si>
+  <si>
+    <t>https://www.deutschebahn.com/en/presse/press_releases/GDL-strike-puts-300-freight-trains-out-of-action--6934016</t>
+  </si>
+  <si>
+    <t>https://logistik-heute.de/news/deutsche-seehaefen-hafenarbeiter-streik-trifft-auf-containerschiff-stau-37141.html</t>
+  </si>
+  <si>
+    <t>https://binnenschifffahrt-online.de/2022/07/featured/26169/tarifkonflikt-hafenarbeiter-streiken-erneut/</t>
+  </si>
+  <si>
+    <t>https://www.reuters.com/business/aerospace-defense/lufthansa-pilots-stage-strike-wage-dispute-2022-09-02/</t>
+  </si>
+  <si>
+    <t>https://www.deutschebahn.com/de/presse/pressestart_zentrales_uebersicht/Presse-Blog-Alle-Infos-zum-GDL-Streik-12467744?</t>
+  </si>
+  <si>
+    <t>https://www.lufthansa-cargo.com/en/-/ver-di-trade-union-strike?</t>
+  </si>
+  <si>
+    <t>https://www.evg-online.org/tarifpolitik/tarifrunde-2023/bundesweiter-warnstreik-der-evg-am-2732023/</t>
+  </si>
+  <si>
+    <t>https://www.verdi.de/presse/pressemitteilungen/%2B%2Bco%2B%2B525d13fc-9f07-11ed-a7fd-001a4a160129</t>
+  </si>
+  <si>
+    <t>https://www.airliners.de/verdi-ruft-lufthansa-cargo-mitarbeiter-streik/73270</t>
   </si>
 </sst>
 </file>
@@ -641,7 +641,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -675,7 +675,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -685,27 +684,17 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -715,32 +704,36 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1081,8 +1074,8 @@
   </sheetPr>
   <dimension ref="A3:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,7 +1087,7 @@
     <col min="5" max="5" width="19" style="5" customWidth="1"/>
     <col min="6" max="6" width="17.140625" style="5" customWidth="1"/>
     <col min="7" max="7" width="100.7109375" customWidth="1"/>
-    <col min="8" max="8" width="19" customWidth="1"/>
+    <col min="8" max="8" width="149.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1115,68 +1108,68 @@
         <v>4</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G5" s="16" t="s">
         <v>2</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="C6" s="6"/>
-      <c r="E6" s="20" t="s">
-        <v>73</v>
+      <c r="E6" s="19" t="s">
+        <v>63</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C7" s="6"/>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="19" t="s">
         <v>3</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14">
+      <c r="A8" s="4">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="F8" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>32</v>
+      <c r="E8" s="17">
+        <v>3</v>
+      </c>
+      <c r="F8" s="5">
+        <v>3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" t="s">
+        <v>10</v>
       </c>
       <c r="I8" s="8" t="str">
         <f>""</f>
@@ -1196,7 +1189,7 @@
       <c r="D9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="17">
         <v>1</v>
       </c>
       <c r="F9" s="9">
@@ -1215,28 +1208,28 @@
     </row>
     <row r="10" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
+        <v>1</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="9">
         <v>9</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="9" t="s">
+      <c r="D10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="17">
         <v>17</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="18">
-        <v>1</v>
-      </c>
       <c r="F10" s="9">
-        <v>1</v>
+        <v>1.9</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>22</v>
+        <v>16</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>5</v>
       </c>
       <c r="I10" t="str">
         <f>""</f>
@@ -1244,29 +1237,29 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
-        <v>11</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="9" t="s">
+      <c r="A11" s="4">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>14</v>
+      <c r="D11" t="s">
+        <v>7</v>
       </c>
       <c r="E11" s="18">
-        <v>1</v>
-      </c>
-      <c r="F11" s="9">
-        <v>1</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>44</v>
+        <v>4</v>
+      </c>
+      <c r="F11" s="5">
+        <v>4</v>
+      </c>
+      <c r="G11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="I11" t="str">
         <f>""</f>
@@ -1274,29 +1267,29 @@
       </c>
     </row>
     <row r="12" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="5" t="s">
+      <c r="A12" s="14">
+        <v>5</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D12" t="s">
-        <v>14</v>
+      <c r="D12" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="E12" s="18">
-        <v>1</v>
-      </c>
-      <c r="F12" s="21">
-        <v>1</v>
-      </c>
-      <c r="G12" t="s">
-        <v>46</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>24</v>
+        <v>28</v>
+      </c>
+      <c r="F12" s="9">
+        <v>28</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="I12" t="str">
         <f>""</f>
@@ -1304,29 +1297,29 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="14">
-        <v>13</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="8" t="s">
+      <c r="A13" s="4">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="5">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="18">
-        <v>1</v>
-      </c>
-      <c r="F13" s="9">
-        <v>1</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>24</v>
+        <v>11</v>
+      </c>
+      <c r="F13" s="5">
+        <v>3.7</v>
+      </c>
+      <c r="G13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>71</v>
       </c>
       <c r="I13" t="str">
         <f>""</f>
@@ -1334,29 +1327,29 @@
       </c>
     </row>
     <row r="14" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="5" t="s">
+      <c r="A14" s="14">
+        <v>7</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="18">
-        <v>1</v>
-      </c>
-      <c r="F14" s="21">
-        <v>1</v>
-      </c>
-      <c r="G14" t="s">
-        <v>50</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>51</v>
+      <c r="D14" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="F14" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>72</v>
       </c>
       <c r="I14" t="str">
         <f>""</f>
@@ -1364,29 +1357,29 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="14">
-        <v>1</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="9">
-        <v>9</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="18">
+      <c r="A15" s="4">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="9">
-        <v>1.9</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="10" t="s">
-        <v>5</v>
+      <c r="D15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="17">
+        <v>2</v>
+      </c>
+      <c r="F15" s="5">
+        <v>2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="I15" t="str">
         <f>""</f>
@@ -1394,29 +1387,29 @@
       </c>
     </row>
     <row r="16" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <v>8</v>
-      </c>
-      <c r="B16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="5" t="s">
+      <c r="A16" s="14">
+        <v>9</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="18">
-        <v>2</v>
-      </c>
-      <c r="F16" s="21">
-        <v>2</v>
-      </c>
-      <c r="G16" t="s">
-        <v>34</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>35</v>
+      <c r="D16" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="17">
+        <v>1</v>
+      </c>
+      <c r="F16" s="9">
+        <v>1</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>74</v>
       </c>
       <c r="I16" t="str">
         <f>""</f>
@@ -1424,29 +1417,29 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
-        <v>10</v>
-      </c>
-      <c r="B17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="5" t="s">
+      <c r="A17" s="14">
+        <v>13</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="18">
-        <v>2</v>
-      </c>
-      <c r="F17" s="21">
-        <v>2</v>
-      </c>
-      <c r="G17" t="s">
-        <v>39</v>
-      </c>
-      <c r="H17" s="7" t="s">
+      <c r="D17" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="17">
+        <v>1</v>
+      </c>
+      <c r="F17" s="9">
+        <v>1</v>
+      </c>
+      <c r="G17" s="8" t="s">
         <v>40</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>75</v>
       </c>
       <c r="I17" t="str">
         <f>""</f>
@@ -1455,28 +1448,28 @@
     </row>
     <row r="18" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="18">
-        <v>3</v>
-      </c>
-      <c r="F18" s="21">
-        <v>3</v>
+        <v>14</v>
+      </c>
+      <c r="E18" s="17">
+        <v>1</v>
+      </c>
+      <c r="F18" s="5">
+        <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" t="s">
-        <v>10</v>
+        <v>39</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="I18" t="str">
         <f>""</f>
@@ -1484,29 +1477,29 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
-        <v>6</v>
-      </c>
-      <c r="B19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="5">
-        <v>3</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="A19" s="14">
+        <v>11</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="19">
-        <v>11</v>
-      </c>
-      <c r="F19" s="21">
-        <v>3.7</v>
-      </c>
-      <c r="G19" t="s">
-        <v>23</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>24</v>
+      <c r="E19" s="17">
+        <v>1</v>
+      </c>
+      <c r="F19" s="9">
+        <v>1</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="I19" t="str">
         <f>""</f>
@@ -1515,28 +1508,28 @@
     </row>
     <row r="20" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="19">
-        <v>4</v>
-      </c>
-      <c r="F20" s="21">
-        <v>4</v>
+        <v>19</v>
+      </c>
+      <c r="E20" s="17">
+        <v>2</v>
+      </c>
+      <c r="F20" s="5">
+        <v>2</v>
       </c>
       <c r="G20" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="I20" t="str">
         <f>""</f>
@@ -1544,29 +1537,29 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="14">
-        <v>5</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="9" t="s">
+      <c r="A21" s="4">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" s="19">
-        <v>28</v>
-      </c>
-      <c r="F21" s="9">
-        <v>28</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>22</v>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="17">
+        <v>1</v>
+      </c>
+      <c r="F21" s="5">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>43</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>79</v>
       </c>
       <c r="I21" t="str">
         <f>""</f>
@@ -1578,170 +1571,164 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E23" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="F23" s="41"/>
-      <c r="G23" s="35"/>
+        <v>52</v>
+      </c>
+      <c r="F23" s="37"/>
+      <c r="G23" s="28"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E24" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="F24" s="37">
+      <c r="E24" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" s="4">
         <f>SUM(E8:E23)</f>
         <v>73.5</v>
       </c>
-      <c r="G24" s="27" t="s">
-        <v>64</v>
+      <c r="G24" s="22" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E25" s="28" t="s">
+      <c r="E25" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" s="29">
+        <v>2.13</v>
+      </c>
+      <c r="G25" s="22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E26" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F25" s="38">
-        <v>2.13</v>
-      </c>
-      <c r="G25" s="27" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E26" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="F26" s="39">
+      <c r="F26" s="30">
         <f>(F24-28-0.5)/22</f>
         <v>2.0454545454545454</v>
       </c>
-      <c r="G26" s="27" t="s">
-        <v>66</v>
+      <c r="G26" s="22" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E27" s="30" t="s">
+      <c r="E27" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="F27" s="31">
+        <v>6.6E-3</v>
+      </c>
+      <c r="G27" s="27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G28" s="38"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G29" s="38"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E30" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="F30" s="35"/>
+      <c r="G30" s="39"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E31" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" s="21">
+        <f>SUM(E8:E18)</f>
+        <v>69.5</v>
+      </c>
+      <c r="G31" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="F27" s="40">
-        <v>6.6E-3</v>
-      </c>
-      <c r="G27" s="32" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G28" s="17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G29" s="42" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E30" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="F30" s="23"/>
-      <c r="G30" s="24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E31" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="F31" s="26">
-        <f>SUM(E8:E18)</f>
-        <v>30.5</v>
-      </c>
-      <c r="G31" s="27" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E32" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="F32" s="29">
+      <c r="E32" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" s="24">
         <v>1.61</v>
       </c>
-      <c r="G32" s="27" t="s">
-        <v>74</v>
+      <c r="G32" s="22" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E33" s="25"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="27"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="22"/>
     </row>
     <row r="34" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E34" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="F34" s="31">
+      <c r="E34" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="F34" s="26">
         <v>5.1999999999999998E-3</v>
       </c>
-      <c r="G34" s="32" t="s">
-        <v>75</v>
+      <c r="G34" s="27" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="5:8" x14ac:dyDescent="0.25">
       <c r="H35" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E37" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="F37" s="34"/>
-      <c r="G37" s="35"/>
+      <c r="E37" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="F37" s="33"/>
+      <c r="G37" s="28"/>
     </row>
     <row r="38" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E38" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="F38" s="26">
+      <c r="E38" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F38" s="21">
         <f>SUM(E19:E21)</f>
-        <v>43</v>
-      </c>
-      <c r="G38" s="27" t="s">
-        <v>72</v>
+        <v>4</v>
+      </c>
+      <c r="G38" s="22" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E39" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="F39" s="29">
+      <c r="E39" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="F39" s="24">
         <v>8.6</v>
       </c>
-      <c r="G39" s="27" t="s">
-        <v>77</v>
+      <c r="G39" s="22" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E40" s="25"/>
-      <c r="F40" s="26"/>
-      <c r="G40" s="27"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E41" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="F41" s="31">
+      <c r="E41" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="F41" s="26">
         <v>1.4E-3</v>
       </c>
-      <c r="G41" s="32" t="s">
-        <v>78</v>
+      <c r="G41" s="27" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A7:H7" xr:uid="{AC7F067A-8AF6-49E2-9E1D-A19C41AAB437}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:H21">
-      <sortCondition ref="F7"/>
+      <sortCondition ref="B7"/>
     </sortState>
   </autoFilter>
   <mergeCells count="3">
@@ -1750,18 +1737,20 @@
     <mergeCell ref="E23:F23"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H15" r:id="rId1" location="Tarifstreit_und_Streiks_2014/2015" xr:uid="{B53E2F89-6395-44B1-9E65-F1ED34C962A1}"/>
-    <hyperlink ref="H20" r:id="rId2" xr:uid="{F8097F3D-1958-4CA3-B87A-CCFB92FBDD05}"/>
-    <hyperlink ref="H21" r:id="rId3" xr:uid="{63F65B85-20D0-45F5-A491-65FF00E05445}"/>
-    <hyperlink ref="H19" r:id="rId4" xr:uid="{12A4E0E6-5E28-42AB-A726-B78B4C537B52}"/>
-    <hyperlink ref="H16" r:id="rId5" xr:uid="{38D2BDBA-D759-470D-A159-9651F03BB6C4}"/>
-    <hyperlink ref="H10" r:id="rId6" xr:uid="{1D747FA6-4944-45F2-BFEE-A75A27CF21DD}"/>
-    <hyperlink ref="H17" r:id="rId7" xr:uid="{0165AAA9-9E60-4052-A9FA-6EA3A9163E75}"/>
-    <hyperlink ref="H12" r:id="rId8" xr:uid="{CB4DFC47-9A51-4744-A89F-55BF729BE327}"/>
-    <hyperlink ref="H13" r:id="rId9" xr:uid="{BE03828C-57B9-44DF-A1C8-E0E82155F763}"/>
-    <hyperlink ref="H14" r:id="rId10" xr:uid="{0BAC5F06-2099-4AF4-88AB-7267E0F748D4}"/>
+    <hyperlink ref="H10" r:id="rId1" location="Tarifstreit_und_Streiks_2014/2015" xr:uid="{B53E2F89-6395-44B1-9E65-F1ED34C962A1}"/>
+    <hyperlink ref="H12" r:id="rId2" xr:uid="{63F65B85-20D0-45F5-A491-65FF00E05445}"/>
+    <hyperlink ref="H13" r:id="rId3" xr:uid="{12A4E0E6-5E28-42AB-A726-B78B4C537B52}"/>
+    <hyperlink ref="H15" r:id="rId4" xr:uid="{38D2BDBA-D759-470D-A159-9651F03BB6C4}"/>
+    <hyperlink ref="H16" r:id="rId5" xr:uid="{1D747FA6-4944-45F2-BFEE-A75A27CF21DD}"/>
+    <hyperlink ref="H20" r:id="rId6" xr:uid="{0165AAA9-9E60-4052-A9FA-6EA3A9163E75}"/>
+    <hyperlink ref="H18" r:id="rId7" xr:uid="{CB4DFC47-9A51-4744-A89F-55BF729BE327}"/>
+    <hyperlink ref="H17" r:id="rId8" xr:uid="{BE03828C-57B9-44DF-A1C8-E0E82155F763}"/>
+    <hyperlink ref="H21" r:id="rId9" xr:uid="{0BAC5F06-2099-4AF4-88AB-7267E0F748D4}"/>
+    <hyperlink ref="H11" r:id="rId10" xr:uid="{D608BCE8-362C-476B-B7B7-E77F5C22C136}"/>
+    <hyperlink ref="H14" r:id="rId11" xr:uid="{749B0290-50ED-4BC3-BDB8-9D120712ACED}"/>
+    <hyperlink ref="H19" r:id="rId12" xr:uid="{DD90A191-A4FC-4270-937C-CEC9B0140784}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="58" orientation="landscape" r:id="rId11"/>
+  <pageSetup scale="58" orientation="landscape" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>